<commit_message>
add 2 tc for evaluating product
</commit_message>
<xml_diff>
--- a/docs/Testcase_Func.xlsx
+++ b/docs/Testcase_Func.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7704" tabRatio="796" firstSheet="13" activeTab="18"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7704" tabRatio="796" firstSheet="12" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Đăng nhập" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="672">
   <si>
     <t>Kiểm thử viên:</t>
   </si>
@@ -3131,6 +3131,38 @@
   <si>
     <t>1. Hiển thị trang chủ của website fahasa.com
 2. Hiển thị "Kết quả tìm kiếm: (10000 sản phẩm)" và có các sản phẩm tên "Detective Conan Zero's Tea Time"</t>
+  </si>
+  <si>
+    <t>TC165</t>
+  </si>
+  <si>
+    <t>Nội dung nhận xét bằng 100 kí tự</t>
+  </si>
+  <si>
+    <t>B1: Mở trình duyệt và truy cập: www.fahasa.com
+B2: Tại ô tìm kiếm nhập: 'Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính'
+B3: Chọn nút "Tìm kiếm" hoặc nhấn Enter
+B4: Chọn sản phẩm có tên: ''Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính''
+B5: Chọn nút "Viết đánh giá"
+B6: Nhập tên đánh giá: 'HienNguyen' và chọn số sao là 2
+B7: Nhập nhận xét về sản phẩm: 'là bộ trò chơi thứ 2 được chuyển thể từ bộ truyện tranh nổi tiếng “Thám tử lừng danh Conan”. Lấy bối' 
+B8: Chọn nút "Gửi nhận xét"</t>
+  </si>
+  <si>
+    <t>TC166</t>
+  </si>
+  <si>
+    <t>Nội dung nhận xét bằng 101 kí tự</t>
+  </si>
+  <si>
+    <t>B1: Mở trình duyệt và truy cập: www.fahasa.com
+B2: Tại ô tìm kiếm nhập: 'Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính'
+B3: Chọn nút "Tìm kiếm" hoặc nhấn Enter
+B4: Chọn sản phẩm có tên: ''Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính''
+B5: Chọn nút "Viết đánh giá"
+B6: Nhập tên đánh giá: 'HienNguyen' và chọn số sao là 2
+B7: Nhập nhận xét về sản phẩm: 'là bộ trò chơi thứ 2 được chuyển thể từ bộ truyện tranh nổi tiếng “Thám tử lừng danh Conan”. Lấy bối c' 
+B8: Chọn nút "Gửi nhận xét"</t>
   </si>
 </sst>
 </file>
@@ -3943,7 +3975,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="118.8" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
         <v>18</v>
       </c>
@@ -3967,7 +3999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="118.8" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
         <v>19</v>
       </c>
@@ -3991,7 +4023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="118.8" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
         <v>20</v>
       </c>
@@ -6492,7 +6524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -7291,10 +7323,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J17"/>
+  <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7524,7 +7556,9 @@
       <c r="D16" s="15" t="s">
         <v>599</v>
       </c>
-      <c r="E16" s="15"/>
+      <c r="E16" s="15" t="s">
+        <v>551</v>
+      </c>
       <c r="F16" s="15" t="s">
         <v>602</v>
       </c>
@@ -7548,7 +7582,9 @@
       <c r="D17" s="15" t="s">
         <v>604</v>
       </c>
-      <c r="E17" s="15"/>
+      <c r="E17" s="15" t="s">
+        <v>551</v>
+      </c>
       <c r="F17" s="15" t="s">
         <v>605</v>
       </c>
@@ -7561,6 +7597,58 @@
       <c r="I17" s="18" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="18" spans="2:9" ht="330" x14ac:dyDescent="0.3">
+      <c r="B18" s="15" t="s">
+        <v>666</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>667</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>551</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>668</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>601</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="330" x14ac:dyDescent="0.3">
+      <c r="B19" s="15" t="s">
+        <v>669</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>670</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>551</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>671</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>601</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D21" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7581,7 +7669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -7793,7 +7881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -7952,7 +8040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -9226,7 +9314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -9550,7 +9638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="277.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="290.39999999999998" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
         <v>218</v>
       </c>

</xml_diff>

<commit_message>
update recharge fpoint script
</commit_message>
<xml_diff>
--- a/docs/Testcase_Func.xlsx
+++ b/docs/Testcase_Func.xlsx
@@ -2853,16 +2853,6 @@
     <t>Nội dung nhận xét nhỏ hơn 100 kí tự</t>
   </si>
   <si>
-    <t>B1: Mở trình duyệt và truy cập: www.fahasa.com
-B2: Tại ô tìm kiếm nhập: 'Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính'
-B3: Chọn nút "Tìm kiếm" hoặc nhấn Enter
-B4: Chọn sản phẩm có tên: ''Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính''
-B5: Chọn nút "Viết đánh giá"
-B6: Nhập tên đánh giá: 'HienNguyen' và chọn số sao là 2
-B7: Nhập nhận xét về sản phẩm: 'là”' 
-B8: Chọn nút "Gửi nhận xét"</t>
-  </si>
-  <si>
     <t>1. Hiển thị trang chủ của website fahasa.com
 2. Hiển thị lịch sử tìm kiếm, từ khóa hot và danh từ nổi bật. Khi nhập tên sản phẩm sẽ hiển thị các từ khóa gợi ý và các sản phẩm có tên tương tự trên mục của thanh tìm kiếm
 3. Hiển thị sách có tên "Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính" và các sản phẩm có tên tương tự
@@ -3139,20 +3129,20 @@
     <t>Nội dung nhận xét bằng 100 kí tự</t>
   </si>
   <si>
+    <t>TC166</t>
+  </si>
+  <si>
+    <t>Nội dung nhận xét bằng 101 kí tự</t>
+  </si>
+  <si>
     <t>B1: Mở trình duyệt và truy cập: www.fahasa.com
 B2: Tại ô tìm kiếm nhập: 'Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính'
 B3: Chọn nút "Tìm kiếm" hoặc nhấn Enter
 B4: Chọn sản phẩm có tên: ''Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính''
 B5: Chọn nút "Viết đánh giá"
 B6: Nhập tên đánh giá: 'HienNguyen' và chọn số sao là 2
-B7: Nhập nhận xét về sản phẩm: 'là bộ trò chơi thứ 2 được chuyển thể từ bộ truyện tranh nổi tiếng “Thám tử lừng danh Conan”. Lấy bối' 
+B7: Nhập nhận xét về sản phẩm: 'là bộ trò chơi thứ 2 được chuyển thể từ bộ truyện tranh nổi tiếng 'Conan - Nàng dâu Halloween: Thính là bộ trò chơi thứ 2 được chuyển thể từ bộ truyện tranh nổi tiếngc' 
 B8: Chọn nút "Gửi nhận xét"</t>
-  </si>
-  <si>
-    <t>TC166</t>
-  </si>
-  <si>
-    <t>Nội dung nhận xét bằng 101 kí tự</t>
   </si>
   <si>
     <t>B1: Mở trình duyệt và truy cập: www.fahasa.com
@@ -3161,7 +3151,17 @@
 B4: Chọn sản phẩm có tên: ''Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính''
 B5: Chọn nút "Viết đánh giá"
 B6: Nhập tên đánh giá: 'HienNguyen' và chọn số sao là 2
-B7: Nhập nhận xét về sản phẩm: 'là bộ trò chơi thứ 2 được chuyển thể từ bộ truyện tranh nổi tiếng “Thám tử lừng danh Conan”. Lấy bối c' 
+B7: Nhập nhận xét về sản phẩm: 'Conan - Nàng dâu Halloween: Thính là bộ trò chơi thứ 2 được chuyển thể từ bộ truyện tranh nổi tiếngcc' 
+B8: Chọn nút "Gửi nhận xét"</t>
+  </si>
+  <si>
+    <t>B1: Mở trình duyệt và truy cập: www.fahasa.com
+B2: Tại ô tìm kiếm nhập: 'Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính'
+B3: Chọn nút "Tìm kiếm" hoặc nhấn Enter
+B4: Chọn sản phẩm có tên: ''Boardgame Thám Tử Lừng Danh Conan - Nàng Dâu Halloween: Thính''
+B5: Chọn nút "Viết đánh giá"
+B6: Nhập tên đánh giá: 'HienNguyen' và chọn số sao là 2
+B7: Nhập nhận xét về sản phẩm: 'Conan - Nàng dâu Halloween: Thính là bộ trò chơi thứ 2 được chuyển thể từ bộ truyện tranh nổi tiếng' 
 B8: Chọn nút "Gửi nhận xét"</t>
   </si>
 </sst>
@@ -4419,7 +4419,7 @@
         <v>370</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F16" s="15" t="s">
         <v>374</v>
@@ -4443,7 +4443,7 @@
         <v>371</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>378</v>
@@ -4465,7 +4465,7 @@
         <v>366</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>376</v>
@@ -4489,7 +4489,7 @@
         <v>367</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>379</v>
@@ -4513,7 +4513,7 @@
         <v>369</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>381</v>
@@ -4537,7 +4537,7 @@
         <v>373</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>383</v>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="22" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
@@ -6022,7 +6022,7 @@
         <v>288</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>523</v>
@@ -7325,8 +7325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7429,7 +7429,7 @@
     </row>
     <row r="11" spans="2:10" ht="184.8" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>14</v>
@@ -7456,7 +7456,7 @@
     </row>
     <row r="12" spans="2:10" ht="171.6" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>14</v>
@@ -7483,7 +7483,7 @@
     </row>
     <row r="13" spans="2:10" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>14</v>
@@ -7522,7 +7522,7 @@
     </row>
     <row r="15" spans="2:10" ht="330" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>14</v>
@@ -7548,7 +7548,7 @@
     </row>
     <row r="16" spans="2:10" ht="316.8" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>14</v>
@@ -7574,7 +7574,7 @@
     </row>
     <row r="17" spans="2:9" ht="303.60000000000002" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>14</v>
@@ -7586,13 +7586,13 @@
         <v>551</v>
       </c>
       <c r="F17" s="15" t="s">
+        <v>671</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>605</v>
       </c>
-      <c r="G17" s="15" t="s">
-        <v>606</v>
-      </c>
       <c r="H17" s="15" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>6</v>
@@ -7600,19 +7600,19 @@
     </row>
     <row r="18" spans="2:9" ht="330" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>551</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="G18" s="15" t="s">
         <v>601</v>
@@ -7623,19 +7623,19 @@
     </row>
     <row r="19" spans="2:9" ht="330" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>551</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G19" s="15" t="s">
         <v>601</v>
@@ -7761,25 +7761,25 @@
     </row>
     <row r="10" spans="2:10" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>358</v>
       </c>
       <c r="F10" s="15" t="s">
+        <v>616</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>617</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>618</v>
-      </c>
       <c r="H10" s="15" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>6</v>
@@ -7788,25 +7788,25 @@
     </row>
     <row r="11" spans="2:10" ht="132" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>358</v>
       </c>
       <c r="F11" s="15" t="s">
+        <v>618</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>619</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>620</v>
-      </c>
       <c r="H11" s="15" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>6</v>
@@ -7815,25 +7815,25 @@
     </row>
     <row r="12" spans="2:10" ht="132" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>358</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>6</v>
@@ -7842,25 +7842,25 @@
     </row>
     <row r="13" spans="2:10" ht="132" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>358</v>
       </c>
       <c r="F13" s="15" t="s">
+        <v>622</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>623</v>
       </c>
-      <c r="G13" s="15" t="s">
-        <v>624</v>
-      </c>
       <c r="H13" s="15" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I13" s="18" t="s">
         <v>6</v>
@@ -7973,25 +7973,25 @@
     </row>
     <row r="10" spans="2:10" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E10" s="15" t="s">
+        <v>633</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>635</v>
-      </c>
       <c r="G10" s="15" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>6</v>
@@ -8000,25 +8000,25 @@
     </row>
     <row r="11" spans="2:10" ht="118.8" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="15" t="s">
+        <v>631</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>632</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>633</v>
-      </c>
       <c r="F11" s="15" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>6</v>
@@ -8132,25 +8132,25 @@
     </row>
     <row r="10" spans="2:10" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>288</v>
       </c>
       <c r="F10" s="15" t="s">
+        <v>637</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>638</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>639</v>
-      </c>
       <c r="H10" s="15" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>6</v>
@@ -8792,13 +8792,13 @@
         <v>358</v>
       </c>
       <c r="F10" s="15" t="s">
+        <v>653</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>654</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>655</v>
-      </c>
       <c r="H10" s="15" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>6</v>
@@ -8817,13 +8817,13 @@
         <v>358</v>
       </c>
       <c r="F11" s="15" t="s">
+        <v>655</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>656</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>657</v>
-      </c>
       <c r="H11" s="15" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>6</v>
@@ -8842,13 +8842,13 @@
         <v>358</v>
       </c>
       <c r="F12" s="15" t="s">
+        <v>657</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>658</v>
       </c>
-      <c r="G12" s="15" t="s">
-        <v>659</v>
-      </c>
       <c r="H12" s="15" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>6</v>
@@ -8866,13 +8866,13 @@
         <v>358</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I13" s="18" t="s">
         <v>6</v>
@@ -8914,13 +8914,13 @@
         <v>358</v>
       </c>
       <c r="F15" s="15" t="s">
+        <v>660</v>
+      </c>
+      <c r="G15" s="15" t="s">
         <v>661</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="H15" s="15" t="s">
         <v>662</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>663</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>6</v>
@@ -8938,13 +8938,13 @@
         <v>358</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>6</v>
@@ -8965,10 +8965,10 @@
         <v>167</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>6</v>
@@ -9406,25 +9406,25 @@
     </row>
     <row r="10" spans="2:10" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>358</v>
       </c>
       <c r="F10" s="15" t="s">
+        <v>644</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>645</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>646</v>
-      </c>
       <c r="H10" s="15" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>6</v>
@@ -9433,25 +9433,25 @@
     </row>
     <row r="11" spans="2:10" ht="105.6" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>358</v>
       </c>
       <c r="F11" s="15" t="s">
+        <v>646</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>647</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>648</v>
-      </c>
       <c r="H11" s="15" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
add forgot password script
</commit_message>
<xml_diff>
--- a/docs/Testcase_Func.xlsx
+++ b/docs/Testcase_Func.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7704" tabRatio="796" firstSheet="12" activeTab="19"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7704" tabRatio="796" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Đăng nhập" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="675">
   <si>
     <t>Kiểm thử viên:</t>
   </si>
@@ -3163,6 +3163,20 @@
 B6: Nhập tên đánh giá: 'HienNguyen' và chọn số sao là 2
 B7: Nhập nhận xét về sản phẩm: 'Conan - Nàng dâu Halloween: Thính là bộ trò chơi thứ 2 được chuyển thể từ bộ truyện tranh nổi tiếng' 
 B8: Chọn nút "Gửi nhận xét"</t>
+  </si>
+  <si>
+    <t>TC167</t>
+  </si>
+  <si>
+    <t>Mã OTP hết hạn</t>
+  </si>
+  <si>
+    <t>1. Hiển thị trang chủ của website fahasa
+2. Hiển thị giao diện Khôi phục mật khẩu
+3. Hiển thị thông báo "OTP đã được gửi" 
+4. Hiển thị thông báo "OTP hợp lệ"
+5. Mở nút "Xác nhận"
+6. Hiển thị thông báo "Mã OTP hết hạn"</t>
   </si>
 </sst>
 </file>
@@ -6855,7 +6869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J24"/>
   <sheetViews>
-    <sheetView zoomScale="117" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="117" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -7325,7 +7339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -8170,10 +8184,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J26"/>
+  <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="96" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8673,9 +8687,32 @@
         <v>6</v>
       </c>
     </row>
+    <row r="27" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
+      <c r="B27" s="15" t="s">
+        <v>672</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>674</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>674</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I10:I26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I10:I27">
       <formula1>"Pass,Failed,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>